<commit_message>
Corrected the wrong date in one cell.
</commit_message>
<xml_diff>
--- a/data/snb-data-snbgwdzid-en-all-20250414_1000.xlsx
+++ b/data/snb-data-snbgwdzid-en-all-20250414_1000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhub1\RStudioProjects\time_series_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CABCD2-E29A-4868-8CE3-45238DDBD265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167769B5-BCEB-4AE0-A4F9-556FC18F1FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6900" yWindow="1920" windowWidth="20265" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5498" uniqueCount="5494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5499" uniqueCount="5494">
   <si>
     <t>SNB data portal</t>
   </si>
@@ -16521,7 +16521,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -16555,6 +16555,12 @@
       <color rgb="FF3E5570"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -16617,7 +16623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -16648,7 +16654,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -16986,7 +16991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O5487"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3952" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A3964" sqref="A3964:A3966"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -17066,75 +17073,75 @@
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
     </row>
     <row r="18" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
     </row>
     <row r="19" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -59186,8 +59193,8 @@
       </c>
     </row>
     <row r="3966" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3966" s="16">
-        <v>43629</v>
+      <c r="A3966" t="s">
+        <v>18</v>
       </c>
       <c r="B3966">
         <v>-0.75</v>
@@ -93080,6 +93087,7 @@
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="C20:E20"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>